<commit_message>
update people-related metrics explanation
</commit_message>
<xml_diff>
--- a/docs/metrics.xlsx
+++ b/docs/metrics.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carloa067660\Documents\Workspace\personal\metricly\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482EB47D-D3D2-4677-A5C0-38E8FD08CA0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B963EEB-05F6-4814-9B38-71C46992C77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E78381C3-C096-4B79-84FA-3CB5B9F855DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E78381C3-C096-4B79-84FA-3CB5B9F855DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
+    <sheet name="People" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="99">
   <si>
     <t>Metrics</t>
   </si>
@@ -159,6 +160,189 @@
   </si>
   <si>
     <t>Interest here in terms of voluntarily giving some of their contact details in exchange for an offer, trial, or more information.</t>
+  </si>
+  <si>
+    <t>Time to Fill</t>
+  </si>
+  <si>
+    <t>Number of days it takes to find and hire a new candidate. Often measured by the number of days between approving a job requisition and the candidate accepting your offer.</t>
+  </si>
+  <si>
+    <t>Staffing Metrics</t>
+  </si>
+  <si>
+    <t>According to Society of Human Resource Management report, a good average time to fill is 42 workdays.</t>
+  </si>
+  <si>
+    <t>Time to Hire</t>
+  </si>
+  <si>
+    <t>Number of days between candidate applies/is approached and when accepts the job.</t>
+  </si>
+  <si>
+    <t>Cost Per Hire</t>
+  </si>
+  <si>
+    <t>Costs associated with the process of hiring new employees. These include expenses such as sourcing and recruitment advertising costs, onboarding, referral bonus program costs.</t>
+  </si>
+  <si>
+    <t>Internal or External Recruiting Cost / Total Number of Hires</t>
+  </si>
+  <si>
+    <t>Internal hiring is the process which company promote or transfer a professional who already works for the company to a new role. Internal hiring cost including administrative (legal document, procedure document, office equipment), training &amp; development, and recruiting staff salary. While external hiring is process hire a professional outside company. External cost including marketing (e.g., cost promote vacany), employee referral cost, job fair expenses.</t>
+  </si>
+  <si>
+    <t>Turnover Rate</t>
+  </si>
+  <si>
+    <t>Percentage of employees leaving in a given period of time (e.g., annual).</t>
+  </si>
+  <si>
+    <t>Number of separation / Avg. number of employees</t>
+  </si>
+  <si>
+    <t>Turnover is when employees are leaving due to dismissal, attrition, and any other reasons.</t>
+  </si>
+  <si>
+    <t>Course Completion Rate</t>
+  </si>
+  <si>
+    <t>How many course completed per employee.</t>
+  </si>
+  <si>
+    <t>Number of employees who completed the courses / Number of employees who enrolled the courses</t>
+  </si>
+  <si>
+    <t>Training &amp; Development Metrics</t>
+  </si>
+  <si>
+    <t>Assessment Pass Rate</t>
+  </si>
+  <si>
+    <t>Rates of employees who passed a course taken.</t>
+  </si>
+  <si>
+    <t>Number of employees who passed the courses / Number of employees who enrolled the courses</t>
+  </si>
+  <si>
+    <t>Training Spend Rates</t>
+  </si>
+  <si>
+    <t>How much of operating costs are attributed to training program.</t>
+  </si>
+  <si>
+    <t>Total training spend / Total operating cost</t>
+  </si>
+  <si>
+    <t>Training Cost Per Employee</t>
+  </si>
+  <si>
+    <t>Average training cost per employee.</t>
+  </si>
+  <si>
+    <t>Total training cost / Number of employee</t>
+  </si>
+  <si>
+    <t>Average Performance Rating</t>
+  </si>
+  <si>
+    <t>Average of performance rating</t>
+  </si>
+  <si>
+    <t>Total all performance ratings / Number of employees who received a performance rating</t>
+  </si>
+  <si>
+    <t>Performance Metrics</t>
+  </si>
+  <si>
+    <t>Performance review is a two-way conversation between manager an employee about performance impact, development, and growth.
+Type of rating scales:
+- Nominal (Which of company values does employee most live-up to? Loyalty/Honesty/Ingenuity/Trust/Accountabilty/Respect)
+- Binary (Is this employee ready for promotion? Yes/No)
+- Ordinal (Poor, Unsatisfactory, Satisfactory, Very Satisfactory, Outstanding)</t>
+  </si>
+  <si>
+    <t>Performance Review Completion Rate</t>
+  </si>
+  <si>
+    <t>Percentage of completed reviews.</t>
+  </si>
+  <si>
+    <t>Number of completed reviews / Number of reviews scheduled</t>
+  </si>
+  <si>
+    <t>Absence Rate</t>
+  </si>
+  <si>
+    <t>Rate of unplanned period of being away from work due to sickness or other causes.</t>
+  </si>
+  <si>
+    <t>Number of absences days / Available working days in given period</t>
+  </si>
+  <si>
+    <t>Promotion Rate</t>
+  </si>
+  <si>
+    <t>Employee promotion is a rate when a company raises a member of its team to higher or more specialized position.</t>
+  </si>
+  <si>
+    <t>Total number of promotion / Number of headcount</t>
+  </si>
+  <si>
+    <t>HR to Employee Worker Ratio</t>
+  </si>
+  <si>
+    <t>Number of HR compared to number of employee working on company.</t>
+  </si>
+  <si>
+    <t>Number of HR / Number of headcount</t>
+  </si>
+  <si>
+    <t>General Workforce Metrics</t>
+  </si>
+  <si>
+    <t>Employee Satisfaction</t>
+  </si>
+  <si>
+    <t>How satisfy an employee is with their job and work environment. To calculate employee satisfaction, company can use these metrics to assess employee satisfaction:
+- Employee NPS
+- Glassdoor.com rating
+- Employee Satisfaction Index (ESI)</t>
+  </si>
+  <si>
+    <t>Employee NPS</t>
+  </si>
+  <si>
+    <t>How likely employee recommend this organization as a place to work.</t>
+  </si>
+  <si>
+    <t>%Promoters - %Detractors</t>
+  </si>
+  <si>
+    <t>Any NPS score that is above 0 is okay. 10-30 is good. Above 59 is excellent. Below -10 is bad.</t>
+  </si>
+  <si>
+    <t>Employee Satisfaction Index (ESI)</t>
+  </si>
+  <si>
+    <t>Usually measured by how satisfied, how well does meet expectations, how close to ideal job. All questions are measured on a scale from 1 to 10.</t>
+  </si>
+  <si>
+    <t>((Question/3) - 1) / 9</t>
+  </si>
+  <si>
+    <t>How satisfied are you with your workplace?
+How well does your workplace meet your expectations?
+How close is your workplace to your ideal job?</t>
+  </si>
+  <si>
+    <t>Salary Hike Since Last Year</t>
+  </si>
+  <si>
+    <t>Annual percentage salary increment.</t>
+  </si>
+  <si>
+    <t>(Current Salary - Previous Year Salary) / Previous Year Salary</t>
   </si>
 </sst>
 </file>
@@ -223,10 +407,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -246,6 +436,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>35730</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1972684</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1381126</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0ADFB97-92AC-4B6F-8ACA-1B70C222B355}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10932330" y="981076"/>
+          <a:ext cx="1936954" cy="1352550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -567,7 +806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{761A02D9-D943-4B88-8C28-EC57E76753AB}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -579,190 +818,490 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2E367C-4669-4786-9373-E6DB780F0BBB}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="68.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="68.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>